<commit_message>
started adding net classes.
</commit_message>
<xml_diff>
--- a/electronics/lcpxpresso-mainboard/pin-allocation.xlsx
+++ b/electronics/lcpxpresso-mainboard/pin-allocation.xlsx
@@ -448,9 +448,6 @@
     <t>silkscreen</t>
   </si>
   <si>
-    <t>rename board</t>
-  </si>
-  <si>
     <t>test all footprints</t>
   </si>
   <si>
@@ -476,6 +473,9 @@
   </si>
   <si>
     <t>add net classes to high voltage lines (spindle, mosfets, etc)</t>
+  </si>
+  <si>
+    <t>finish routing all signals</t>
   </si>
 </sst>
 </file>
@@ -566,7 +566,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="93">
+  <cellStyleXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -660,8 +660,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -679,8 +681,9 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="93">
+  <cellStyles count="95">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -727,6 +730,7 @@
     <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -773,6 +777,7 @@
     <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1105,7 +1110,7 @@
   <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1412,17 +1417,17 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>142</v>
+        <v>150</v>
       </c>
     </row>
     <row r="22" spans="1:4">
-      <c r="A22" t="s">
-        <v>143</v>
+      <c r="A22" s="9" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -1627,7 +1632,7 @@
         <v>83</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -1653,7 +1658,7 @@
         <v>85</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -1679,7 +1684,7 @@
         <v>86</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -1731,7 +1736,7 @@
         <v>87</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -1757,7 +1762,7 @@
         <v>88</v>
       </c>
       <c r="K12" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -1803,7 +1808,7 @@
         <v>90</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -1826,7 +1831,7 @@
         <v>91</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="16" spans="1:11">

</xml_diff>

<commit_message>
worked more on footprints and added to the hoekstep17 setup.
</commit_message>
<xml_diff>
--- a/electronics/lcpxpresso-mainboard/pin-allocation.xlsx
+++ b/electronics/lcpxpresso-mainboard/pin-allocation.xlsx
@@ -472,10 +472,10 @@
     <t>SPINDLE RELAY</t>
   </si>
   <si>
-    <t>add net classes to high voltage lines (spindle, mosfets, etc)</t>
-  </si>
-  <si>
-    <t>finish routing all signals</t>
+    <t>add config jumpers for hoekstep drivers</t>
+  </si>
+  <si>
+    <t>look into routing DAC into ROSC pins on hoekstep</t>
   </si>
 </sst>
 </file>
@@ -663,7 +663,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -681,7 +681,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="95">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1110,7 +1109,7 @@
   <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1417,22 +1416,22 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
     </row>
     <row r="22" spans="1:4">
-      <c r="A22" s="9" t="s">
-        <v>151</v>
+      <c r="A22" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>142</v>
+        <v>150</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>141</v>
+        <v>151</v>
       </c>
     </row>
   </sheetData>
@@ -1450,7 +1449,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView topLeftCell="A23" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added mode set pins and started work on routing the AOUT signal.
</commit_message>
<xml_diff>
--- a/electronics/lcpxpresso-mainboard/pin-allocation.xlsx
+++ b/electronics/lcpxpresso-mainboard/pin-allocation.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="151">
   <si>
     <t>Pin Name</t>
   </si>
@@ -472,10 +472,7 @@
     <t>SPINDLE RELAY</t>
   </si>
   <si>
-    <t>add config jumpers for hoekstep drivers</t>
-  </si>
-  <si>
-    <t>look into routing DAC into ROSC pins on hoekstep</t>
+    <t>toggle around pins to route AOUT (P0.26) to VREF</t>
   </si>
 </sst>
 </file>
@@ -1106,10 +1103,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="A23" sqref="A23:XFD23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1427,11 +1424,6 @@
     <row r="23" spans="1:4">
       <c r="A23" t="s">
         <v>150</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
-      <c r="A24" t="s">
-        <v>151</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
toggled pins around, finished routing, tidied up silkscreen, and checked for drc errors.
</commit_message>
<xml_diff>
--- a/electronics/lcpxpresso-mainboard/pin-allocation.xlsx
+++ b/electronics/lcpxpresso-mainboard/pin-allocation.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="150">
   <si>
     <t>Pin Name</t>
   </si>
@@ -445,9 +445,6 @@
     <t>more todo:</t>
   </si>
   <si>
-    <t>silkscreen</t>
-  </si>
-  <si>
     <t>test all footprints</t>
   </si>
   <si>
@@ -472,7 +469,7 @@
     <t>SPINDLE RELAY</t>
   </si>
   <si>
-    <t>toggle around pins to route AOUT (P0.26) to VREF</t>
+    <t>VOUT</t>
   </si>
 </sst>
 </file>
@@ -563,8 +560,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="95">
+  <cellStyleXfs count="103">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -679,7 +684,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="95">
+  <cellStyles count="103">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -727,6 +732,10 @@
     <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -774,6 +783,10 @@
     <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1103,10 +1116,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:XFD23"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1413,17 +1426,7 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="A22" t="s">
         <v>141</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
-      <c r="A23" t="s">
-        <v>150</v>
       </c>
     </row>
   </sheetData>
@@ -1441,8 +1444,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1623,7 +1626,7 @@
         <v>83</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -1649,7 +1652,7 @@
         <v>85</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -1675,7 +1678,7 @@
         <v>86</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -1727,7 +1730,7 @@
         <v>87</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -1753,7 +1756,7 @@
         <v>88</v>
       </c>
       <c r="K12" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -1799,7 +1802,7 @@
         <v>90</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -1822,7 +1825,7 @@
         <v>91</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -1833,7 +1836,7 @@
         <v>10</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>138</v>
+        <v>149</v>
       </c>
       <c r="E16" t="s">
         <v>76</v>
@@ -1856,7 +1859,7 @@
         <v>10</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>108</v>
+        <v>138</v>
       </c>
       <c r="E17" t="s">
         <v>77</v>
@@ -1886,6 +1889,9 @@
       </c>
       <c r="I18" t="s">
         <v>94</v>
+      </c>
+      <c r="K18" s="4" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="19" spans="1:11">

</xml_diff>